<commit_message>
Deploying to gh-pages from @ eurovibes/ws2813-breakout@70aee180076696aa3aaede84f0b52b7f4eeace9b 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/ws2813-breakout-bom_.xlsx
+++ b/Fabrication/BoM/ws2813-breakout-bom_.xlsx
@@ -164,7 +164,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2021-09-26_17-42-51</t>
+    <t>2021-09-26_18-56-52</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -347,9 +347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1316740</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>63248</xdr:rowOff>
+      <xdr:colOff>2399886</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>56736</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -367,7 +367,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2231140" cy="1225298"/>
+          <a:ext cx="3314286" cy="3314286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>